<commit_message>
Allow to Save without interaction
</commit_message>
<xml_diff>
--- a/Test_Intk_Book.xlsx
+++ b/Test_Intk_Book.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\MyScripts_uc\vb\Excel_Referral_Intk_2016\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\MyScripts_uc\vb\Excel_Referral_Intk_2016\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D53487C-AD0C-4C67-80E7-9BA70B3FDCF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6999544F-B31B-46E1-BB94-8B806DF0CB59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35100" yWindow="2055" windowWidth="18900" windowHeight="10965" xr2:uid="{68AE8EDB-3EA2-49D2-820B-9BE0B46D776D}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{68AE8EDB-3EA2-49D2-820B-9BE0B46D776D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,14 +22,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t>Test 3</t>
-  </si>
-</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -384,13 +376,7 @@
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Customized from Test to start making it functional.
</commit_message>
<xml_diff>
--- a/Test_Intk_Book.xlsx
+++ b/Test_Intk_Book.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\MyScripts_uc\vb\Excel_Referral_Intk_2016\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6999544F-B31B-46E1-BB94-8B806DF0CB59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{689918FC-9070-4D2D-BCAD-55BBBA3C49BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{68AE8EDB-3EA2-49D2-820B-9BE0B46D776D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{68AE8EDB-3EA2-49D2-820B-9BE0B46D776D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,11 +24,63 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+  <si>
+    <t xml:space="preserve">Child Name: </t>
+  </si>
+  <si>
+    <t>LEA:</t>
+  </si>
+  <si>
+    <t>Offense(s):</t>
+  </si>
+  <si>
+    <t>Case No:</t>
+  </si>
+  <si>
+    <t>Status:</t>
+  </si>
+  <si>
+    <t>Intake Completed:</t>
+  </si>
+  <si>
+    <t>Case Received Date:</t>
+  </si>
+  <si>
+    <t>Days Pending:</t>
+  </si>
+  <si>
+    <t>Last Case Status Date:</t>
+  </si>
+  <si>
+    <t>Threshold:</t>
+  </si>
+  <si>
+    <t>Days Till Next Threshold</t>
+  </si>
+  <si>
+    <t>Intake Status Sheet</t>
+  </si>
+  <si>
+    <t>Progress Notes:</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="24"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -43,7 +95,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -51,12 +103,62 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -371,12 +473,130 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49D9058B-F519-464E-A0FC-A60109C20571}">
-  <dimension ref="A1"/>
+  <dimension ref="A2:L6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="25.5703125" style="10" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" style="8" customWidth="1"/>
+    <col min="3" max="3" width="25.28515625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" style="8" customWidth="1"/>
+    <col min="5" max="5" width="19.140625" style="8" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.42578125" style="8" customWidth="1"/>
+    <col min="9" max="9" width="15" style="8" customWidth="1"/>
+    <col min="10" max="10" width="11.7109375" style="8" customWidth="1"/>
+    <col min="11" max="11" width="11.42578125" style="8" customWidth="1"/>
+    <col min="12" max="12" width="34.42578125" style="13" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:12" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A2" s="4"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="12"/>
+    </row>
+    <row r="3" spans="1:12" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A3" s="4"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="14"/>
+    </row>
+    <row r="4" spans="1:12" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="5"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="15"/>
+      <c r="K4" s="15"/>
+      <c r="L4" s="15"/>
+    </row>
+    <row r="5" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G6" s="9"/>
+      <c r="H6" s="8" t="str">
+        <f ca="1">IF(G6&gt;0,_xlfn.DAYS(TODAY(), G6) &amp; " Days", "")</f>
+        <v/>
+      </c>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9" t="str">
+        <f>IF(I6&gt;0, I6+30, "")</f>
+        <v/>
+      </c>
+      <c r="K6" s="8" t="str">
+        <f ca="1">IF(I6&gt;0,SUM(J6-TODAY()) &amp; " Days","")</f>
+        <v/>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C3:L4"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Solved finding last blank row.
</commit_message>
<xml_diff>
--- a/Test_Intk_Book.xlsx
+++ b/Test_Intk_Book.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\MyScripts_uc\vb\Excel_Referral_Intk_2016\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{689918FC-9070-4D2D-BCAD-55BBBA3C49BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F00EC979-5BC0-4C90-B406-7A7D95074D50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{68AE8EDB-3EA2-49D2-820B-9BE0B46D776D}"/>
   </bookViews>
@@ -473,16 +473,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49D9058B-F519-464E-A0FC-A60109C20571}">
-  <dimension ref="A2:L6"/>
+  <dimension ref="A2:L40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.5703125" style="10" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" style="8" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" style="8" customWidth="1"/>
     <col min="3" max="3" width="25.28515625" style="3" customWidth="1"/>
     <col min="4" max="4" width="15.85546875" style="8" customWidth="1"/>
     <col min="5" max="5" width="19.140625" style="8" customWidth="1"/>
@@ -593,6 +593,484 @@
         <v/>
       </c>
     </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G7" s="9"/>
+      <c r="H7" s="8" t="str">
+        <f t="shared" ref="H7:H40" ca="1" si="0">IF(G7&gt;0,_xlfn.DAYS(TODAY(), G7) &amp; " Days", "")</f>
+        <v/>
+      </c>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9" t="str">
+        <f t="shared" ref="J7:J40" si="1">IF(I7&gt;0, I7+30, "")</f>
+        <v/>
+      </c>
+      <c r="K7" s="8" t="str">
+        <f t="shared" ref="K7:K40" ca="1" si="2">IF(I7&gt;0,SUM(J7-TODAY()) &amp; " Days","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H8" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v/>
+      </c>
+      <c r="J8" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K8" s="8" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H9" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v/>
+      </c>
+      <c r="J9" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K9" s="8" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H10" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v/>
+      </c>
+      <c r="J10" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K10" s="8" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H11" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v/>
+      </c>
+      <c r="J11" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K11" s="8" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H12" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v/>
+      </c>
+      <c r="J12" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K12" s="8" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H13" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v/>
+      </c>
+      <c r="J13" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K13" s="8" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H14" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v/>
+      </c>
+      <c r="J14" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K14" s="8" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H15" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v/>
+      </c>
+      <c r="J15" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K15" s="8" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H16" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v/>
+      </c>
+      <c r="J16" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K16" s="8" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H17" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v/>
+      </c>
+      <c r="J17" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K17" s="8" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H18" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v/>
+      </c>
+      <c r="J18" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K18" s="8" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H19" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v/>
+      </c>
+      <c r="J19" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K19" s="8" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H20" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v/>
+      </c>
+      <c r="J20" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K20" s="8" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H21" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v/>
+      </c>
+      <c r="J21" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K21" s="8" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H22" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v/>
+      </c>
+      <c r="J22" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K22" s="8" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="23" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H23" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v/>
+      </c>
+      <c r="J23" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K23" s="8" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="24" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H24" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v/>
+      </c>
+      <c r="J24" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K24" s="8" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="25" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H25" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v/>
+      </c>
+      <c r="J25" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K25" s="8" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="26" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H26" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v/>
+      </c>
+      <c r="J26" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K26" s="8" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="27" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H27" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v/>
+      </c>
+      <c r="J27" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K27" s="8" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="28" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H28" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v/>
+      </c>
+      <c r="J28" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K28" s="8" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="29" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H29" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v/>
+      </c>
+      <c r="J29" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K29" s="8" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="30" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H30" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v/>
+      </c>
+      <c r="J30" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K30" s="8" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="31" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H31" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v/>
+      </c>
+      <c r="J31" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K31" s="8" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="32" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H32" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v/>
+      </c>
+      <c r="J32" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K32" s="8" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="33" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H33" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v/>
+      </c>
+      <c r="J33" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K33" s="8" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="34" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H34" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v/>
+      </c>
+      <c r="J34" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K34" s="8" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="35" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H35" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v/>
+      </c>
+      <c r="J35" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K35" s="8" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="36" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H36" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v/>
+      </c>
+      <c r="J36" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K36" s="8" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="37" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H37" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v/>
+      </c>
+      <c r="J37" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K37" s="8" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="38" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H38" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v/>
+      </c>
+      <c r="J38" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K38" s="8" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="39" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H39" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v/>
+      </c>
+      <c r="J39" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K39" s="8" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="40" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H40" s="8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v/>
+      </c>
+      <c r="J40" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="K40" s="8" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="C3:L4"/>

</xml_diff>

<commit_message>
Added New Law Enforcement
Added new agencies that were missing.
</commit_message>
<xml_diff>
--- a/Test_Intk_Book.xlsx
+++ b/Test_Intk_Book.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\MyScripts_uc\vb\Excel_Projects\Excel_Intk_Ref_2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D23B8F29-0752-499E-B94F-68FC35188441}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E89B7BE9-DB5C-40E5-9CF7-3AFA9F596C13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30750" yWindow="1950" windowWidth="24180" windowHeight="11295" xr2:uid="{68AE8EDB-3EA2-49D2-820B-9BE0B46D776D}"/>
   </bookViews>
@@ -600,7 +600,7 @@
   <dimension ref="A2:L41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:L4"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>